<commit_message>
Updated Specs & Backend Logics
</commit_message>
<xml_diff>
--- a/Specifications (仕様書)/BD (基本設計)/Database.xlsx
+++ b/Specifications (仕様書)/BD (基本設計)/Database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng quan" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="78">
   <si>
     <t>Tác giả:</t>
   </si>
@@ -89,9 +89,6 @@
     <t>not null</t>
   </si>
   <si>
-    <t>MAX</t>
-  </si>
-  <si>
     <t>GioiTinh</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>Tên chức vụ</t>
+  </si>
+  <si>
+    <t>Phường</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -775,10 +775,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -811,7 +811,9 @@
       <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
@@ -826,19 +828,19 @@
       <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>21</v>
+      <c r="E7" s="7">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>20</v>
@@ -847,13 +849,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>20</v>
@@ -862,10 +864,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>19</v>
@@ -879,118 +881,118 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>21</v>
+      <c r="E11" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>21</v>
+      <c r="E12" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="C13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>21</v>
+      <c r="E13" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>21</v>
+      <c r="E14" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
+      </c>
+      <c r="E15" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>21</v>
+      <c r="E16" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="C17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="7">
         <v>20</v>
@@ -998,33 +1000,33 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
+      </c>
+      <c r="E18" s="7">
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="7">
         <v>20</v>
@@ -1032,16 +1034,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="C20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="7">
         <v>128</v>
@@ -1049,18 +1051,20 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="E21" s="7">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1069,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E19"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1090,15 +1094,15 @@
         <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1131,17 +1135,19 @@
       <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>20</v>
@@ -1150,13 +1156,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>20</v>
@@ -1165,13 +1171,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>20</v>
@@ -1180,10 +1186,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>19</v>
@@ -1197,27 +1203,27 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>21</v>
+      <c r="E11" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>19</v>
@@ -1225,16 +1231,16 @@
       <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>21</v>
+      <c r="E12" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>19</v>
@@ -1242,88 +1248,111 @@
       <c r="D13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>21</v>
+      <c r="E13" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="E15" s="7">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
+      </c>
+      <c r="E16" s="7">
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="E17" s="7">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="E18" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="7">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1354,15 +1383,15 @@
         <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1399,16 +1428,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5">
         <v>20</v>
@@ -1443,15 +1472,15 @@
         <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1476,7 +1505,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>15</v>
@@ -1488,16 +1517,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5">
         <v>30</v>

</xml_diff>